<commit_message>
Add not equal token. Add CountIf formula and tests
</commit_message>
<xml_diff>
--- a/src/ExcelCompiler.Net.Readers.Tests/Data/tests.xlsx
+++ b/src/ExcelCompiler.Net.Readers.Tests/Data/tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HenrikStengaard\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\First Realize\ExcelCompiler.Net\src\ExcelCompiler.Net.Readers.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2603661-D09A-4315-BD3F-EE1657BB4F1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC99A735-FFF4-4167-9176-D5F063BD8E6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F4715D3D-C4EC-4F2C-A193-644ED03A7D86}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{F4715D3D-C4EC-4F2C-A193-644ED03A7D86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="20">
   <si>
     <t>A</t>
   </si>
@@ -82,6 +76,15 @@
   </si>
   <si>
     <t>Two numeric values</t>
+  </si>
+  <si>
+    <t>InRange</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Has Value</t>
   </si>
 </sst>
 </file>
@@ -442,18 +445,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C096BE-8C94-4A8A-9CFC-AC53E3341503}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -467,7 +470,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -482,7 +485,7 @@
         <v>True</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -497,7 +500,7 @@
         <v>False</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -512,7 +515,7 @@
         <v>True</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -527,7 +530,7 @@
         <v>False</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -542,7 +545,7 @@
         <v>True</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -557,7 +560,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -572,7 +575,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -587,7 +590,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -602,7 +605,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -616,7 +619,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -631,7 +634,7 @@
         <v>False</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -646,7 +649,7 @@
         <v>False</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -661,7 +664,7 @@
         <v>False</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -676,7 +679,7 @@
         <v>True</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -691,7 +694,7 @@
         <v>True</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -706,7 +709,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -721,7 +724,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -736,7 +739,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -751,7 +754,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
@@ -765,7 +768,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -777,7 +780,7 @@
         <v>False</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -789,7 +792,7 @@
         <v>True</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -801,7 +804,7 @@
         <v>True</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -813,7 +816,7 @@
         <v>False</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -825,7 +828,7 @@
         <v>False</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -837,7 +840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -849,7 +852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -861,7 +864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -873,7 +876,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>16</v>
       </c>
@@ -887,7 +890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -902,7 +905,7 @@
         <v>False</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -917,7 +920,7 @@
         <v>True</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -932,7 +935,7 @@
         <v>True</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -947,7 +950,7 @@
         <v>False</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -962,7 +965,7 @@
         <v>False</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -977,7 +980,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -992,7 +995,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -1007,7 +1010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -1020,6 +1023,42 @@
       <c r="D43">
         <f>B43/C43</f>
         <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <f>COUNTIF(B46:B48,C46)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B48">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>